<commit_message>
Add support for reading and writing rich text #9
</commit_message>
<xml_diff>
--- a/tests/xlsx/image_nao.xlsx
+++ b/tests/xlsx/image_nao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\edit-xlsx\tests\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pt/Projects/Github/edit-xlsx/tests/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EF83C6-08F0-41DF-9230-CC89772FCE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37500B13-13E6-424D-98A6-EFEC2610E20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,22 +24,117 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+      </rPr>
+      <t>H</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+      </rPr>
+      <t>E</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>O</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,11 +157,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -401,12 +497,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="53" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>